<commit_message>
Update blacklist.xlsx with new data
</commit_message>
<xml_diff>
--- a/data/blacklist.xlsx
+++ b/data/blacklist.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\steel-flower-blacklist\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B91851-42FE-4B9A-BD85-C0F3DDA3928B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F408C8F4-3C1D-429D-82B0-AF2BECB3D842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
   <si>
     <t>In-Game Name</t>
   </si>
@@ -52,9 +52,6 @@
     <t>auraisme666</t>
   </si>
   <si>
-    <t>8.272406766672937e+17</t>
-  </si>
-  <si>
     <t>Permananet</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t>brutallyy</t>
   </si>
   <si>
-    <t>8.32491214673543e+17</t>
-  </si>
-  <si>
     <t>Permanent</t>
   </si>
   <si>
@@ -91,9 +85,6 @@
     <t>kerdi3333</t>
   </si>
   <si>
-    <t>1.2779947538787901e+18</t>
-  </si>
-  <si>
     <t>Hacking</t>
   </si>
   <si>
@@ -106,9 +97,6 @@
     <t>deleted_user6467</t>
   </si>
   <si>
-    <t>3.8143946876413536e+17</t>
-  </si>
-  <si>
     <t>Permanently Banned in-game.</t>
   </si>
   <si>
@@ -121,9 +109,6 @@
     <t>kerdi6666</t>
   </si>
   <si>
-    <t>8.373571292700344e+17</t>
-  </si>
-  <si>
     <t>Inactive</t>
   </si>
   <si>
@@ -145,19 +130,10 @@
     <t>struesenberg</t>
   </si>
   <si>
-    <t>7.23479360379551e+17</t>
-  </si>
-  <si>
     <t>Patchouli</t>
   </si>
   <si>
-    <t>137534547</t>
-  </si>
-  <si>
     <t>hikamarine</t>
-  </si>
-  <si>
-    <t>173312357244600320</t>
   </si>
   <si>
     <t>N/A</t>
@@ -171,7 +147,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -222,12 +198,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,7 +511,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,202 +555,204 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>8.2724067666729306E+17</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>165851335</v>
       </c>
       <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4">
+        <v>8.3249121467354304E+17</v>
+      </c>
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>205945394</v>
       </c>
       <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1.2779947538787899E+18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
         <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B5">
         <v>158347339</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3.8143946876413498E+17</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <v>238568279</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" t="s">
-        <v>33</v>
+        <v>28</v>
+      </c>
+      <c r="D6" s="4">
+        <v>8.3735712927003405E+17</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B7">
         <v>229930708</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="2">
-        <v>45771.74722222222</v>
+        <v>33</v>
+      </c>
+      <c r="H7" s="2" t="str">
+        <f>TEXT(DATE(2025,4,25) + TIME(17,49,0), "yyyy-mm-dd hh:mm")</f>
+        <v>2025-04-25 17:49</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B8">
         <v>175510531</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" t="s">
-        <v>41</v>
+        <v>35</v>
+      </c>
+      <c r="D8" s="4">
+        <v>7.2347936037955098E+17</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" s="2">
-        <v>45771.742361111108</v>
+        <v>33</v>
+      </c>
+      <c r="H8" s="2" t="str">
+        <f>TEXT(DATE(2025,4,24) + TIME(17,49,0), "yyyy-mm-dd hh:mm")</f>
+        <v>2025-04-24 17:49</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" t="s">
-        <v>43</v>
+        <v>36</v>
+      </c>
+      <c r="B9" s="3">
+        <v>137534547</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" t="s">
-        <v>45</v>
+        <v>37</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.733123572446E+17</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H9" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update app.py, blacklist.xlsx with new fixes
</commit_message>
<xml_diff>
--- a/data/blacklist.xlsx
+++ b/data/blacklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\steel-flower-blacklist\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F408C8F4-3C1D-429D-82B0-AF2BECB3D842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A846C0-5CAD-41F0-89C9-37BF0C517C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -198,13 +198,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -511,7 +510,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,7 +580,7 @@
       <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>8.3249121467354304E+17</v>
       </c>
       <c r="E3" t="s">
@@ -607,7 +606,7 @@
       <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>1.2779947538787899E+18</v>
       </c>
       <c r="E4" t="s">
@@ -633,7 +632,7 @@
       <c r="C5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>3.8143946876413498E+17</v>
       </c>
       <c r="E5" t="s">
@@ -659,7 +658,7 @@
       <c r="C6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>8.3735712927003405E+17</v>
       </c>
       <c r="E6" t="s">
@@ -712,7 +711,7 @@
       <c r="C8" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>7.2347936037955098E+17</v>
       </c>
       <c r="E8" t="s">
@@ -733,13 +732,13 @@
       <c r="A9" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9">
         <v>137534547</v>
       </c>
       <c r="C9" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9">
         <v>1.733123572446E+17</v>
       </c>
       <c r="E9" t="s">

</xml_diff>